<commit_message>
before Drholmes  meeting update
</commit_message>
<xml_diff>
--- a/Validation/model_metrics_summary.xlsx
+++ b/Validation/model_metrics_summary.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/smncd_umsystem_edu/Documents/MS_T/Research/LRF_RC/Validation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD3F0D57C93358491453088B35299F657" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A777DB3D-5E66-482B-B244-914A62FFCB92}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,8 +61,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,7 +73,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,14 +125,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -423,22 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -481,104 +462,104 @@
         <v>0.999745545652451</v>
       </c>
       <c r="C2">
-        <v>0.99974561038299514</v>
+        <v>0.9997456103829951</v>
       </c>
       <c r="D2">
-        <v>7455895.9634168567</v>
+        <v>7455895.963416857</v>
       </c>
       <c r="E2">
-        <v>1825.2626222153051</v>
+        <v>1825.262622215305</v>
       </c>
       <c r="F2">
-        <v>0.99374007354434801</v>
+        <v>0.993740073544348</v>
       </c>
       <c r="G2">
-        <v>0.99992768604693893</v>
+        <v>0.9999276860469389</v>
       </c>
       <c r="H2">
-        <v>0.69420199933685023</v>
+        <v>0.6942019993368502</v>
       </c>
       <c r="I2">
-        <v>0.69420199933685023</v>
+        <v>0.6942019993368502</v>
       </c>
       <c r="J2">
-        <v>0.31274180003619212</v>
+        <v>0.3127418000361921</v>
       </c>
       <c r="K2">
         <v>106822</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>0.99908374819460721</v>
+        <v>0.9990837481946072</v>
       </c>
       <c r="C3">
-        <v>0.99908458694347302</v>
+        <v>0.999084586943473</v>
       </c>
       <c r="D3">
         <v>26847559.11268042</v>
       </c>
       <c r="E3">
-        <v>4562.6012316042743</v>
+        <v>4562.601231604274</v>
       </c>
       <c r="F3">
-        <v>0.98129370160763929</v>
+        <v>0.9812937016076393</v>
       </c>
       <c r="G3">
-        <v>0.99973960833962749</v>
+        <v>0.9997396083396275</v>
       </c>
       <c r="H3">
-        <v>1.9751569917405489</v>
+        <v>1.975156991740549</v>
       </c>
       <c r="I3">
-        <v>1.9751569917405489</v>
+        <v>1.975156991740549</v>
       </c>
       <c r="J3">
-        <v>0.59345585021273872</v>
+        <v>0.5934558502127387</v>
       </c>
       <c r="K3">
         <v>106822</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
-        <v>0.99979968914572204</v>
+        <v>0.999799689145722</v>
       </c>
       <c r="C4">
-        <v>0.99979972926212479</v>
+        <v>0.9997997292621248</v>
       </c>
       <c r="D4">
-        <v>5869409.9913225183</v>
+        <v>5869409.991322518</v>
       </c>
       <c r="E4">
         <v>1875.320824200069</v>
       </c>
       <c r="F4">
-        <v>0.99347575329820348</v>
+        <v>0.9934757532982035</v>
       </c>
       <c r="G4">
-        <v>0.99994307320801001</v>
+        <v>0.99994307320801</v>
       </c>
       <c r="H4">
-        <v>0.79228571876255771</v>
+        <v>0.7922857187625577</v>
       </c>
       <c r="I4">
-        <v>0.79228571876255771</v>
+        <v>0.7922857187625577</v>
       </c>
       <c r="J4">
-        <v>0.27748098998235149</v>
+        <v>0.2774809899823515</v>
       </c>
       <c r="K4">
         <v>106822</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update before new machine
</commit_message>
<xml_diff>
--- a/Validation/model_metrics_summary.xlsx
+++ b/Validation/model_metrics_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sheet</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Method_3</t>
+  </si>
+  <si>
+    <t>Method</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,6 +562,41 @@
         <v>106822</v>
       </c>
     </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.9949715634984005</v>
+      </c>
+      <c r="C5">
+        <v>0.9949967221633021</v>
+      </c>
+      <c r="D5">
+        <v>147340769.6732198</v>
+      </c>
+      <c r="E5">
+        <v>5509.050019388131</v>
+      </c>
+      <c r="F5">
+        <v>0.9634307661821588</v>
+      </c>
+      <c r="G5">
+        <v>0.9985709573263347</v>
+      </c>
+      <c r="H5">
+        <v>1.361060513652995</v>
+      </c>
+      <c r="I5">
+        <v>1.361060513652995</v>
+      </c>
+      <c r="J5">
+        <v>1.390264645806614</v>
+      </c>
+      <c r="K5">
+        <v>106822</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>